<commit_message>
Updating figure 1 and table 1
</commit_message>
<xml_diff>
--- a/results/Potential table 1 (summary expectations and key points).xlsx
+++ b/results/Potential table 1 (summary expectations and key points).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Oilcontent_Longevity/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{A2E00401-D436-4788-82E8-B5DE3D85093D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58935EF7-D55A-4F53-9354-7F70E62849C7}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{A2E00401-D436-4788-82E8-B5DE3D85093D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED384239-1BE5-4DA5-ADC0-E8465AD07347}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CC793E85-7B50-438A-B7CD-80EF6DDB8885}"/>
   </bookViews>
@@ -36,46 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
-  <si>
-    <t>UFA</t>
-  </si>
-  <si>
-    <t>SFA</t>
-  </si>
-  <si>
-    <t>production cost</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>energy stored</t>
-  </si>
-  <si>
-    <t>melting point</t>
-  </si>
-  <si>
-    <t>oxidative damage</t>
-  </si>
-  <si>
-    <t>extra</t>
-  </si>
-  <si>
-    <t>less palatable</t>
-  </si>
-  <si>
-    <t>antifreezer (up to -5ºC)</t>
-  </si>
-  <si>
-    <t>Fatty acids biochemical properties</t>
-  </si>
-  <si>
-    <t>Small seeds should maximize SFA but that is not the case</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Oil content</t>
   </si>
@@ -224,51 +185,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -286,6 +239,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -605,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC7ADD2-5251-4D0D-8C0F-F29AFE34753F}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,217 +577,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>14</v>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="4" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A16:B16"/>
+  <mergeCells count="6">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>